<commit_message>
Added conditional formating for average marks greater than 50
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -53,7 +53,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,7 +386,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>99</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -394,7 +394,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>95</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -402,7 +402,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -410,8 +410,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <f>AVERAGE(B1:B4)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>